<commit_message>
replaced mathjax with svg files in model landing pages
</commit_message>
<xml_diff>
--- a/utils/model2json/ca_information.xlsx
+++ b/utils/model2json/ca_information.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="356" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="356" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -529,58 +529,58 @@
     <t>utility function</t>
   </si>
   <si>
-    <t>sum_{t=0}^{\\infty }\\beta ^{t}\\left[ \\frac{\\left( c_{t}-\\varkappa c_{t-1}\\right) ^{1-\\gamma }}{1-\\gamma }+\\kappa \\frac{\\left( g_{t}-\\varkappa g_{t-1}\\right) ^{1-\\gamma }}{1-\\gamma }\\right]</t>
+    <t>\sum_{t=0}^{\infty }\beta ^{t}\left[ \frac{\left( c_{t}-\varkappa c_{t-1}\right) ^{1-\gamma }}{1-\gamma }+\kappa \frac{\left( g_{t}-\varkappa g_{t-1}\right) ^{1-\gamma }}{1-\gamma }\right]</t>
   </si>
   <si>
     <t>long run growth rate</t>
   </si>
   <si>
-    <t>$(1+%\\mathfrak{g})=(1+\\mathfrak{g}_{a})(1+\\mathfrak{g}_{n})$</t>
+    <t>(1+\mathfrak{g})=(1+\mathfrak{g}_{a})(1+\mathfrak{g}_{n})</t>
   </si>
   <si>
     <t>production function of non-oil sector</t>
   </si>
   <si>
-    <t>y_{t}^{n}=ak_{t-1}^{\\theta _{k}}s_{t-1}^{\\theta _{s}}</t>
+    <t>y_{t}^{n}=ak_{t-1}^{\theta _{k}}s_{t-1}^{\theta _{s}}</t>
   </si>
   <si>
     <t>public capital accumulation</t>
   </si>
   <si>
-    <t>(1+\\mathfrak{g})s_{t+1}=e_{s}i_{t}^{s}+(1-\\delta _{s})s_{t}</t>
+    <t>(1+\mathfrak{g})s_{t+1}=e_{s}i_{t}^{s}+(1-\delta _{s})s_{t}</t>
   </si>
   <si>
     <t>investment inefficiency</t>
   </si>
   <si>
-    <t>(1+\\mathfrak{g})k_{t+1}=e_{k}i_{t}^{k}+(1-\\delta _{k})k_{t}</t>
+    <t>(1+\mathfrak{g})k_{t+1}=e_{k}i_{t}^{k}+(1-\delta _{k})k_{t}</t>
   </si>
   <si>
     <t>public capital adjustment cost</t>
   </si>
   <si>
-    <t>AC_{t}^{s}=\\frac{\\phi _{s}}{2}\\left( \\frac{s_{t}}{s_{t-1}}-1\\right) ^{2}s_{t-1}</t>
+    <t>AC_{t}^{s}=\frac{\phi _{s}}{2}\left( \frac{s_{t}}{s_{t-1}}-1\right) ^{2}s_{t-1}</t>
   </si>
   <si>
     <t>private capital adjustment cost</t>
   </si>
   <si>
-    <t>AC_{t}^{k}=\\frac{\\phi _{k}}{2}\\left( \\frac{k_{t}}{k_{t-1}}-1\\right) ^{2}k_{t-1}</t>
+    <t>AC_{t}^{k}=\frac{\phi _{k}}{2}\left( \frac{k_{t}}{k_{t-1}}-1\right) ^{2}k_{t-1}</t>
   </si>
   <si>
     <t>premium</t>
   </si>
   <si>
-    <t>Pi (d_{t})=r_{t}-r^{\\ast }=\\frac{\\pi }{\\rho _{1}^{2}}\\left[ e^{\\rho _{1}(d_{t}-\\bar{d}-\\psi V_{t})}-\\rho _{2}(d_{t}-\\overline{d}-\\psi V_{t})-\\rho _{3}\\right]</t>
-  </si>
-  <si>
-    <t>ca_{t}=d_{t-1}-(1+\\mathfrak{g})d_{t}</t>
+    <t>\Pi (d_{t})=r_{t}-r^{\ast }=\frac{\pi }{\rho _{1}^{2}}\left[ e^{\rho _{1}(d_{t}-\bar{d}-\psi V_{t})}-\rho _{2}(d_{t}-\overline{d}-\psi V_{t})-\rho _{3}\right]</t>
+  </si>
+  <si>
+    <t>ca_{t}=d_{t-1}-(1+\mathfrak{g})d_{t}</t>
   </si>
   <si>
     <t>resource constraint of the economy</t>
   </si>
   <si>
-    <t>(1+\\mathfrak{g})d_{t}=(1+r_{t-1})d_{t-1}+c_{t}+i_{t}^{k}+AC_{t}^{k}+g_{t}+i_{t}^{s}+AC_{t}^{s}+i_{t}^{o}-y_{t}^{n}-y_{t}^{o}-T_{t}</t>
+    <t>(1+\mathfrak{g})d_{t}=(1+r_{t-1})d_{t-1}+c_{t}+i_{t}^{k}+AC_{t}^{k}+g_{t}+i_{t}^{s}+AC_{t}^{s}+i_{t}^{o}-y_{t}^{n}-y_{t}^{o}-T_{t}</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1014,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1714,8 +1714,8 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
add svgs for params
</commit_message>
<xml_diff>
--- a/utils/model2json/ca_information.xlsx
+++ b/utils/model2json/ca_information.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="356" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="356" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -175,7 +175,7 @@
     <t>theta_k</t>
   </si>
   <si>
-    <t>\\theta_{k}</t>
+    <t>\theta_{k}</t>
   </si>
   <si>
     <t>ratio of private capital</t>
@@ -190,7 +190,7 @@
     <t>theta_s</t>
   </si>
   <si>
-    <t>\\theta_{s}</t>
+    <t>\theta_{s}</t>
   </si>
   <si>
     <t>ratio of public capital</t>
@@ -202,7 +202,7 @@
     <t>gamma</t>
   </si>
   <si>
-    <t>\\gamma</t>
+    <t>\gamma</t>
   </si>
   <si>
     <t>risk aversion rate</t>
@@ -217,7 +217,7 @@
     <t>delta_k</t>
   </si>
   <si>
-    <t>\\delta_{k}</t>
+    <t>\delta_{k}</t>
   </si>
   <si>
     <t>depreciation rate of private capital</t>
@@ -229,7 +229,7 @@
     <t>delta_s</t>
   </si>
   <si>
-    <t>\\delta_{s}</t>
+    <t>\delta_{s}</t>
   </si>
   <si>
     <t>depreciation rate of public capital</t>
@@ -241,7 +241,7 @@
     <t>rbar</t>
   </si>
   <si>
-    <t>\\bar{r}</t>
+    <t>\bar{r}</t>
   </si>
   <si>
     <t>world interest rate</t>
@@ -298,7 +298,7 @@
     <t>dbar</t>
   </si>
   <si>
-    <t>\\bar{d}</t>
+    <t>\bar{d}</t>
   </si>
   <si>
     <t>steady state debt</t>
@@ -310,7 +310,7 @@
     <t>xi</t>
   </si>
   <si>
-    <t>\\varkappa</t>
+    <t>\varkappa</t>
   </si>
   <si>
     <t>habit persistence parameter</t>
@@ -322,7 +322,7 @@
     <t>rho1</t>
   </si>
   <si>
-    <t>\\rho_{1}</t>
+    <t>\rho_{1}</t>
   </si>
   <si>
     <t>interest rate-debt elasticity</t>
@@ -334,7 +334,7 @@
     <t>rho2</t>
   </si>
   <si>
-    <t>\\rho_{2}</t>
+    <t>\rho_{2}</t>
   </si>
   <si>
     <t>additional parameter on risk-premium</t>
@@ -343,7 +343,7 @@
     <t>psi</t>
   </si>
   <si>
-    <t>\\psi</t>
+    <t>\psi</t>
   </si>
   <si>
     <t>between 0 and 1</t>
@@ -367,7 +367,7 @@
     <t>omega</t>
   </si>
   <si>
-    <t>\\omega</t>
+    <t>\omega</t>
   </si>
   <si>
     <t>leverage coefficient on oil reserves</t>
@@ -400,7 +400,7 @@
     <t>itermax</t>
   </si>
   <si>
-    <t>\\text{itermax}</t>
+    <t>\text{itermax}</t>
   </si>
   <si>
     <t>Determines the maximum number of iterations used in the non-linear solver. The default value of maxit is 10. The maxit option is shared with the steady command. So a change in maxit in asimul command will also be considered in the following steady commands.</t>
@@ -514,7 +514,7 @@
     <t>gov_exp_0</t>
   </si>
   <si>
-    <t>gov_exp_{0}</t>
+    <t>govexp_{0}</t>
   </si>
   <si>
     <t>gov total expenditure in percent of GDP</t>
@@ -1467,8 +1467,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1714,7 +1714,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>